<commit_message>
Data updated with the new results
</commit_message>
<xml_diff>
--- a/data/Non_local_games_data.xlsx
+++ b/data/Non_local_games_data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuele Dalla Torre\Dropbox\Bell Graph Inequalities\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4A6BD3-FFAE-4277-BC89-3BF23D9D68C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB99A26-A3FD-4FF9-B28F-DC481B08DBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="ionq" sheetId="2" r:id="rId2"/>
     <sheet name="IBM-melbourne" sheetId="3" r:id="rId3"/>
     <sheet name="IBM-boeblingen" sheetId="5" r:id="rId4"/>
-    <sheet name="honeywell" sheetId="6" r:id="rId5"/>
-    <sheet name="ionq-55" sheetId="7" r:id="rId6"/>
+    <sheet name="honeywell-H0" sheetId="6" r:id="rId5"/>
+    <sheet name="honeywell-H1" sheetId="8" r:id="rId6"/>
+    <sheet name="ionq-optima-mermin" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataSignature="AMtx7mhcqfQmYMS4LxBDR0RdhCvgZdwlvg=="/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>System</t>
   </si>
@@ -153,6 +151,12 @@
   <si>
     <t>18/04/21 bis</t>
   </si>
+  <si>
+    <t>Honeywell h1</t>
+  </si>
+  <si>
+    <t>Honeywell h0</t>
+  </si>
 </sst>
 </file>
 
@@ -204,7 +208,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +219,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -254,6 +264,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,23 +516,23 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
@@ -1076,37 +1090,37 @@
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="9">
-        <f t="shared" ref="B13:E13" si="0">AVERAGE(B5:B12)</f>
+        <f>AVERAGE(B5:B12)</f>
         <v>37.5</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(C5:C12)</f>
         <v>84.75</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5:D12)</f>
         <v>83.287500000000009</v>
       </c>
       <c r="E13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E5:E12)</f>
         <v>42.5506591796875</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9">
-        <f t="shared" ref="H13:K13" si="1">AVERAGE(H5:H12)</f>
+        <f>AVERAGE(H5:H12)</f>
         <v>82.862499999999997</v>
       </c>
       <c r="I13" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(I5:I12)</f>
         <v>80.375</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(J5:J12)</f>
         <v>75.287500000000009</v>
       </c>
       <c r="K13" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(K5:K12)</f>
         <v>81.737499999999997</v>
       </c>
       <c r="L13" s="5"/>
@@ -1555,35 +1569,35 @@
     <row r="22" spans="1:29" ht="15.75" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="9">
-        <f t="shared" ref="B22:I22" si="2">AVERAGE(B14:B21)</f>
+        <f t="shared" ref="B22:I22" si="0">AVERAGE(B14:B21)</f>
         <v>37.5</v>
       </c>
       <c r="C22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>84.11454067185106</v>
       </c>
       <c r="D22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>85.744699289182293</v>
       </c>
       <c r="E22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>57.676433750000008</v>
       </c>
       <c r="F22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>78.80663527134989</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>83.554526608485489</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>88.612641475772847</v>
       </c>
       <c r="I22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>83.969100090490855</v>
       </c>
       <c r="J22" s="9">
@@ -2905,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2919,12 +2933,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
@@ -3104,19 +3118,19 @@
     </row>
     <row r="13" spans="1:6" ht="12" customHeight="1">
       <c r="A13" s="9">
-        <f t="shared" ref="A13:D13" si="0">AVERAGE(A5:A12)</f>
+        <f>AVERAGE(A5:A12)</f>
         <v>82.862499999999997</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B5:B12)</f>
         <v>80.375</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(C5:C12)</f>
         <v>75.287500000000009</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5:D12)</f>
         <v>81.737499999999997</v>
       </c>
       <c r="E13" s="5"/>
@@ -3258,11 +3272,11 @@
     </row>
     <row r="22" spans="1:6" ht="12" customHeight="1">
       <c r="A22" s="9">
-        <f t="shared" ref="A22:B22" si="1">AVERAGE(A14:A21)</f>
+        <f>AVERAGE(A14:A21)</f>
         <v>88.612641475772847</v>
       </c>
       <c r="B22" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(B14:B21)</f>
         <v>83.969100090490855</v>
       </c>
       <c r="C22" s="9">
@@ -4864,11 +4878,11 @@
       <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:15" ht="12" customHeight="1">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -6375,10 +6389,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="12" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" ht="12" customHeight="1">
       <c r="A2" s="7">
@@ -6512,11 +6526,11 @@
     </row>
     <row r="22" spans="1:4" ht="12" customHeight="1">
       <c r="A22" s="9">
-        <f t="shared" ref="A22:B22" si="0">AVERAGE(A14:A21)</f>
+        <f>AVERAGE(A14:A21)</f>
         <v>78.80663527134989</v>
       </c>
       <c r="B22" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B14:B21)</f>
         <v>83.554526608485489</v>
       </c>
       <c r="C22" s="5"/>
@@ -7570,21 +7584,22 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="15"/>
+      <c r="A1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
@@ -7595,7 +7610,9 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="15">
+        <v>44343</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1">
@@ -7605,7 +7622,9 @@
       <c r="B3" s="6">
         <v>1000</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5">
+        <v>1024</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1">
@@ -7615,7 +7634,7 @@
       <c r="B4" s="3">
         <v>417</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1">
@@ -7625,7 +7644,9 @@
       <c r="B5" s="1">
         <v>81.099999999999994</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="14">
+        <v>0.8994140625</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1">
@@ -7635,7 +7656,9 @@
       <c r="B6" s="1">
         <v>88</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="14">
+        <v>0.9541015625</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1">
@@ -7645,7 +7668,9 @@
       <c r="B7" s="1">
         <v>87.9</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="14">
+        <v>0.951171875</v>
+      </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1">
@@ -7655,7 +7680,9 @@
       <c r="B8" s="1">
         <v>79.2</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="14">
+        <v>0.90625</v>
+      </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="12" customHeight="1">
@@ -7665,7 +7692,9 @@
       <c r="B9" s="1">
         <v>85.9</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="14">
+        <v>0.9638671875</v>
+      </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1">
@@ -7675,7 +7704,9 @@
       <c r="B10" s="1">
         <v>78.3</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="14">
+        <v>0.900390625</v>
+      </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="12" customHeight="1">
@@ -7685,7 +7716,9 @@
       <c r="B11" s="1">
         <v>78.2</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="14">
+        <v>0.900390625</v>
+      </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="12" customHeight="1">
@@ -7695,22 +7728,27 @@
       <c r="B12" s="1">
         <v>87.7</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="14">
+        <v>0.9404296875</v>
+      </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1">
       <c r="A13" s="9">
-        <f t="shared" ref="A13:B13" si="0">AVERAGE(A5:A12)</f>
+        <f>AVERAGE(A5:A12)</f>
         <v>84.75</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B5:B12)</f>
         <v>83.287500000000009</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="9">
+        <f>100*AVERAGE(C5:C12)</f>
+        <v>92.7001953125</v>
+      </c>
       <c r="D13" s="1">
-        <f>AVERAGE(A13:B13)</f>
-        <v>84.018750000000011</v>
+        <f>AVERAGE(A13:C13)</f>
+        <v>86.912565104166674</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1">
@@ -7722,8 +7760,8 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="1">
-        <f>_xlfn.STDEV.P(A13:B13)</f>
-        <v>0.73124999999999574</v>
+        <f>_xlfn.STDEV.P(A13:C13)</f>
+        <v>4.135796911020444</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1">
@@ -7798,11 +7836,11 @@
     </row>
     <row r="22" spans="1:4" ht="12" customHeight="1">
       <c r="A22" s="9">
-        <f t="shared" ref="A22:B22" si="1">AVERAGE(A14:A21)</f>
+        <f>AVERAGE(A14:A21)</f>
         <v>84.11454067185106</v>
       </c>
       <c r="B22" s="9">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(B14:B21)</f>
         <v>85.744699289182293</v>
       </c>
       <c r="C22" s="5"/>
@@ -8852,10 +8890,1191 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1240785B-7A91-4148-A8B4-148014F4D850}">
+  <dimension ref="A1:D1000"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="20" style="14" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="14" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" style="14" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="12" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="12" customHeight="1">
+      <c r="A2" s="16">
+        <v>44343</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="12" customHeight="1">
+      <c r="A3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="12" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="12" customHeight="1">
+      <c r="A5" s="1">
+        <v>0.9609375</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.95703125</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.9716796875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12" customHeight="1">
+      <c r="A6" s="1">
+        <v>0.9794921875</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.98046875</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.974609375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="12" customHeight="1">
+      <c r="A7" s="1">
+        <v>0.9794921875</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.978515625</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.9755859375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12" customHeight="1">
+      <c r="A8" s="1">
+        <v>0.9716796875</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.955078125</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0.9580078125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12" customHeight="1">
+      <c r="A9" s="1">
+        <v>0.9775390625</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.97265625</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0.974609375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="12" customHeight="1">
+      <c r="A10" s="1">
+        <v>0.9697265625</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.955078125</v>
+      </c>
+      <c r="C10" s="17">
+        <v>0.9580078125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12" customHeight="1">
+      <c r="A11" s="1">
+        <v>0.962890625</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.955078125</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.9560546875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="12" customHeight="1">
+      <c r="A12" s="1">
+        <v>0.9794921875</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.974609375</v>
+      </c>
+      <c r="C12" s="17">
+        <v>0.978515625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="12" customHeight="1">
+      <c r="A13" s="9">
+        <f>AVERAGE(A5:A12)</f>
+        <v>0.97265625</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" ref="B13:C13" si="0">AVERAGE(B5:B12)</f>
+        <v>0.966064453125</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9683837890625</v>
+      </c>
+      <c r="D13" s="1">
+        <f>AVERAGE(A13:C13)</f>
+        <v>0.96903483072916663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12" customHeight="1">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="1">
+        <f>STDEV(A13:C13)</f>
+        <v>3.3437760016360282E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="12" customHeight="1">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="12" customHeight="1">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" ht="12" customHeight="1">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="12" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="12" customHeight="1">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="12" customHeight="1">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="12" customHeight="1">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="12" customHeight="1">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="D22" s="1" t="e">
+        <f>AVERAGE(A22:B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12" customHeight="1">
+      <c r="D23" s="1" t="e">
+        <f>_xlfn.STDEV.P(A22:B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12" customHeight="1"/>
+    <row r="25" spans="1:4" ht="12" customHeight="1"/>
+    <row r="26" spans="1:4" ht="12" customHeight="1"/>
+    <row r="27" spans="1:4" ht="12" customHeight="1"/>
+    <row r="28" spans="1:4" ht="12" customHeight="1"/>
+    <row r="29" spans="1:4" ht="12" customHeight="1"/>
+    <row r="30" spans="1:4" ht="12" customHeight="1"/>
+    <row r="31" spans="1:4" ht="12" customHeight="1"/>
+    <row r="32" spans="1:4" ht="12" customHeight="1"/>
+    <row r="33" ht="12" customHeight="1"/>
+    <row r="34" ht="12" customHeight="1"/>
+    <row r="35" ht="12" customHeight="1"/>
+    <row r="36" ht="12" customHeight="1"/>
+    <row r="37" ht="12" customHeight="1"/>
+    <row r="38" ht="12" customHeight="1"/>
+    <row r="39" ht="12" customHeight="1"/>
+    <row r="40" ht="12" customHeight="1"/>
+    <row r="41" ht="12" customHeight="1"/>
+    <row r="42" ht="12" customHeight="1"/>
+    <row r="43" ht="12" customHeight="1"/>
+    <row r="44" ht="12" customHeight="1"/>
+    <row r="45" ht="12" customHeight="1"/>
+    <row r="46" ht="12" customHeight="1"/>
+    <row r="47" ht="12" customHeight="1"/>
+    <row r="48" ht="12" customHeight="1"/>
+    <row r="49" ht="12" customHeight="1"/>
+    <row r="50" ht="12" customHeight="1"/>
+    <row r="51" ht="12" customHeight="1"/>
+    <row r="52" ht="12" customHeight="1"/>
+    <row r="53" ht="12" customHeight="1"/>
+    <row r="54" ht="12" customHeight="1"/>
+    <row r="55" ht="12" customHeight="1"/>
+    <row r="56" ht="12" customHeight="1"/>
+    <row r="57" ht="12" customHeight="1"/>
+    <row r="58" ht="12" customHeight="1"/>
+    <row r="59" ht="12" customHeight="1"/>
+    <row r="60" ht="12" customHeight="1"/>
+    <row r="61" ht="12" customHeight="1"/>
+    <row r="62" ht="12" customHeight="1"/>
+    <row r="63" ht="12" customHeight="1"/>
+    <row r="64" ht="12" customHeight="1"/>
+    <row r="65" ht="12" customHeight="1"/>
+    <row r="66" ht="12" customHeight="1"/>
+    <row r="67" ht="12" customHeight="1"/>
+    <row r="68" ht="12" customHeight="1"/>
+    <row r="69" ht="12" customHeight="1"/>
+    <row r="70" ht="12" customHeight="1"/>
+    <row r="71" ht="12" customHeight="1"/>
+    <row r="72" ht="12" customHeight="1"/>
+    <row r="73" ht="12" customHeight="1"/>
+    <row r="74" ht="12" customHeight="1"/>
+    <row r="75" ht="12" customHeight="1"/>
+    <row r="76" ht="12" customHeight="1"/>
+    <row r="77" ht="12" customHeight="1"/>
+    <row r="78" ht="12" customHeight="1"/>
+    <row r="79" ht="12" customHeight="1"/>
+    <row r="80" ht="12" customHeight="1"/>
+    <row r="81" ht="12" customHeight="1"/>
+    <row r="82" ht="12" customHeight="1"/>
+    <row r="83" ht="12" customHeight="1"/>
+    <row r="84" ht="12" customHeight="1"/>
+    <row r="85" ht="12" customHeight="1"/>
+    <row r="86" ht="12" customHeight="1"/>
+    <row r="87" ht="12" customHeight="1"/>
+    <row r="88" ht="12" customHeight="1"/>
+    <row r="89" ht="12" customHeight="1"/>
+    <row r="90" ht="12" customHeight="1"/>
+    <row r="91" ht="12" customHeight="1"/>
+    <row r="92" ht="12" customHeight="1"/>
+    <row r="93" ht="12" customHeight="1"/>
+    <row r="94" ht="12" customHeight="1"/>
+    <row r="95" ht="12" customHeight="1"/>
+    <row r="96" ht="12" customHeight="1"/>
+    <row r="97" ht="12" customHeight="1"/>
+    <row r="98" ht="12" customHeight="1"/>
+    <row r="99" ht="12" customHeight="1"/>
+    <row r="100" ht="12" customHeight="1"/>
+    <row r="101" ht="12" customHeight="1"/>
+    <row r="102" ht="12" customHeight="1"/>
+    <row r="103" ht="12" customHeight="1"/>
+    <row r="104" ht="12" customHeight="1"/>
+    <row r="105" ht="12" customHeight="1"/>
+    <row r="106" ht="12" customHeight="1"/>
+    <row r="107" ht="12" customHeight="1"/>
+    <row r="108" ht="12" customHeight="1"/>
+    <row r="109" ht="12" customHeight="1"/>
+    <row r="110" ht="12" customHeight="1"/>
+    <row r="111" ht="12" customHeight="1"/>
+    <row r="112" ht="12" customHeight="1"/>
+    <row r="113" ht="12" customHeight="1"/>
+    <row r="114" ht="12" customHeight="1"/>
+    <row r="115" ht="12" customHeight="1"/>
+    <row r="116" ht="12" customHeight="1"/>
+    <row r="117" ht="12" customHeight="1"/>
+    <row r="118" ht="12" customHeight="1"/>
+    <row r="119" ht="12" customHeight="1"/>
+    <row r="120" ht="12" customHeight="1"/>
+    <row r="121" ht="12" customHeight="1"/>
+    <row r="122" ht="12" customHeight="1"/>
+    <row r="123" ht="12" customHeight="1"/>
+    <row r="124" ht="12" customHeight="1"/>
+    <row r="125" ht="12" customHeight="1"/>
+    <row r="126" ht="12" customHeight="1"/>
+    <row r="127" ht="12" customHeight="1"/>
+    <row r="128" ht="12" customHeight="1"/>
+    <row r="129" ht="12" customHeight="1"/>
+    <row r="130" ht="12" customHeight="1"/>
+    <row r="131" ht="12" customHeight="1"/>
+    <row r="132" ht="12" customHeight="1"/>
+    <row r="133" ht="12" customHeight="1"/>
+    <row r="134" ht="12" customHeight="1"/>
+    <row r="135" ht="12" customHeight="1"/>
+    <row r="136" ht="12" customHeight="1"/>
+    <row r="137" ht="12" customHeight="1"/>
+    <row r="138" ht="12" customHeight="1"/>
+    <row r="139" ht="12" customHeight="1"/>
+    <row r="140" ht="12" customHeight="1"/>
+    <row r="141" ht="12" customHeight="1"/>
+    <row r="142" ht="12" customHeight="1"/>
+    <row r="143" ht="12" customHeight="1"/>
+    <row r="144" ht="12" customHeight="1"/>
+    <row r="145" ht="12" customHeight="1"/>
+    <row r="146" ht="12" customHeight="1"/>
+    <row r="147" ht="12" customHeight="1"/>
+    <row r="148" ht="12" customHeight="1"/>
+    <row r="149" ht="12" customHeight="1"/>
+    <row r="150" ht="12" customHeight="1"/>
+    <row r="151" ht="12" customHeight="1"/>
+    <row r="152" ht="12" customHeight="1"/>
+    <row r="153" ht="12" customHeight="1"/>
+    <row r="154" ht="12" customHeight="1"/>
+    <row r="155" ht="12" customHeight="1"/>
+    <row r="156" ht="12" customHeight="1"/>
+    <row r="157" ht="12" customHeight="1"/>
+    <row r="158" ht="12" customHeight="1"/>
+    <row r="159" ht="12" customHeight="1"/>
+    <row r="160" ht="12" customHeight="1"/>
+    <row r="161" ht="12" customHeight="1"/>
+    <row r="162" ht="12" customHeight="1"/>
+    <row r="163" ht="12" customHeight="1"/>
+    <row r="164" ht="12" customHeight="1"/>
+    <row r="165" ht="12" customHeight="1"/>
+    <row r="166" ht="12" customHeight="1"/>
+    <row r="167" ht="12" customHeight="1"/>
+    <row r="168" ht="12" customHeight="1"/>
+    <row r="169" ht="12" customHeight="1"/>
+    <row r="170" ht="12" customHeight="1"/>
+    <row r="171" ht="12" customHeight="1"/>
+    <row r="172" ht="12" customHeight="1"/>
+    <row r="173" ht="12" customHeight="1"/>
+    <row r="174" ht="12" customHeight="1"/>
+    <row r="175" ht="12" customHeight="1"/>
+    <row r="176" ht="12" customHeight="1"/>
+    <row r="177" ht="12" customHeight="1"/>
+    <row r="178" ht="12" customHeight="1"/>
+    <row r="179" ht="12" customHeight="1"/>
+    <row r="180" ht="12" customHeight="1"/>
+    <row r="181" ht="12" customHeight="1"/>
+    <row r="182" ht="12" customHeight="1"/>
+    <row r="183" ht="12" customHeight="1"/>
+    <row r="184" ht="12" customHeight="1"/>
+    <row r="185" ht="12" customHeight="1"/>
+    <row r="186" ht="12" customHeight="1"/>
+    <row r="187" ht="12" customHeight="1"/>
+    <row r="188" ht="12" customHeight="1"/>
+    <row r="189" ht="12" customHeight="1"/>
+    <row r="190" ht="12" customHeight="1"/>
+    <row r="191" ht="12" customHeight="1"/>
+    <row r="192" ht="12" customHeight="1"/>
+    <row r="193" ht="12" customHeight="1"/>
+    <row r="194" ht="12" customHeight="1"/>
+    <row r="195" ht="12" customHeight="1"/>
+    <row r="196" ht="12" customHeight="1"/>
+    <row r="197" ht="12" customHeight="1"/>
+    <row r="198" ht="12" customHeight="1"/>
+    <row r="199" ht="12" customHeight="1"/>
+    <row r="200" ht="12" customHeight="1"/>
+    <row r="201" ht="12" customHeight="1"/>
+    <row r="202" ht="12" customHeight="1"/>
+    <row r="203" ht="12" customHeight="1"/>
+    <row r="204" ht="12" customHeight="1"/>
+    <row r="205" ht="12" customHeight="1"/>
+    <row r="206" ht="12" customHeight="1"/>
+    <row r="207" ht="12" customHeight="1"/>
+    <row r="208" ht="12" customHeight="1"/>
+    <row r="209" ht="12" customHeight="1"/>
+    <row r="210" ht="12" customHeight="1"/>
+    <row r="211" ht="12" customHeight="1"/>
+    <row r="212" ht="12" customHeight="1"/>
+    <row r="213" ht="12" customHeight="1"/>
+    <row r="214" ht="12" customHeight="1"/>
+    <row r="215" ht="12" customHeight="1"/>
+    <row r="216" ht="12" customHeight="1"/>
+    <row r="217" ht="12" customHeight="1"/>
+    <row r="218" ht="12" customHeight="1"/>
+    <row r="219" ht="12" customHeight="1"/>
+    <row r="220" ht="12" customHeight="1"/>
+    <row r="221" ht="12" customHeight="1"/>
+    <row r="222" ht="12" customHeight="1"/>
+    <row r="223" ht="12" customHeight="1"/>
+    <row r="224" ht="12" customHeight="1"/>
+    <row r="225" ht="12" customHeight="1"/>
+    <row r="226" ht="12" customHeight="1"/>
+    <row r="227" ht="12" customHeight="1"/>
+    <row r="228" ht="12" customHeight="1"/>
+    <row r="229" ht="12" customHeight="1"/>
+    <row r="230" ht="12" customHeight="1"/>
+    <row r="231" ht="12" customHeight="1"/>
+    <row r="232" ht="12" customHeight="1"/>
+    <row r="233" ht="12" customHeight="1"/>
+    <row r="234" ht="12" customHeight="1"/>
+    <row r="235" ht="12" customHeight="1"/>
+    <row r="236" ht="12" customHeight="1"/>
+    <row r="237" ht="12" customHeight="1"/>
+    <row r="238" ht="12" customHeight="1"/>
+    <row r="239" ht="12" customHeight="1"/>
+    <row r="240" ht="12" customHeight="1"/>
+    <row r="241" ht="12" customHeight="1"/>
+    <row r="242" ht="12" customHeight="1"/>
+    <row r="243" ht="12" customHeight="1"/>
+    <row r="244" ht="12" customHeight="1"/>
+    <row r="245" ht="12" customHeight="1"/>
+    <row r="246" ht="12" customHeight="1"/>
+    <row r="247" ht="12" customHeight="1"/>
+    <row r="248" ht="12" customHeight="1"/>
+    <row r="249" ht="12" customHeight="1"/>
+    <row r="250" ht="12" customHeight="1"/>
+    <row r="251" ht="12" customHeight="1"/>
+    <row r="252" ht="12" customHeight="1"/>
+    <row r="253" ht="12" customHeight="1"/>
+    <row r="254" ht="12" customHeight="1"/>
+    <row r="255" ht="12" customHeight="1"/>
+    <row r="256" ht="12" customHeight="1"/>
+    <row r="257" ht="12" customHeight="1"/>
+    <row r="258" ht="12" customHeight="1"/>
+    <row r="259" ht="12" customHeight="1"/>
+    <row r="260" ht="12" customHeight="1"/>
+    <row r="261" ht="12" customHeight="1"/>
+    <row r="262" ht="12" customHeight="1"/>
+    <row r="263" ht="12" customHeight="1"/>
+    <row r="264" ht="12" customHeight="1"/>
+    <row r="265" ht="12" customHeight="1"/>
+    <row r="266" ht="12" customHeight="1"/>
+    <row r="267" ht="12" customHeight="1"/>
+    <row r="268" ht="12" customHeight="1"/>
+    <row r="269" ht="12" customHeight="1"/>
+    <row r="270" ht="12" customHeight="1"/>
+    <row r="271" ht="12" customHeight="1"/>
+    <row r="272" ht="12" customHeight="1"/>
+    <row r="273" ht="12" customHeight="1"/>
+    <row r="274" ht="12" customHeight="1"/>
+    <row r="275" ht="12" customHeight="1"/>
+    <row r="276" ht="12" customHeight="1"/>
+    <row r="277" ht="12" customHeight="1"/>
+    <row r="278" ht="12" customHeight="1"/>
+    <row r="279" ht="12" customHeight="1"/>
+    <row r="280" ht="12" customHeight="1"/>
+    <row r="281" ht="12" customHeight="1"/>
+    <row r="282" ht="12" customHeight="1"/>
+    <row r="283" ht="12" customHeight="1"/>
+    <row r="284" ht="12" customHeight="1"/>
+    <row r="285" ht="12" customHeight="1"/>
+    <row r="286" ht="12" customHeight="1"/>
+    <row r="287" ht="12" customHeight="1"/>
+    <row r="288" ht="12" customHeight="1"/>
+    <row r="289" ht="12" customHeight="1"/>
+    <row r="290" ht="12" customHeight="1"/>
+    <row r="291" ht="12" customHeight="1"/>
+    <row r="292" ht="12" customHeight="1"/>
+    <row r="293" ht="12" customHeight="1"/>
+    <row r="294" ht="12" customHeight="1"/>
+    <row r="295" ht="12" customHeight="1"/>
+    <row r="296" ht="12" customHeight="1"/>
+    <row r="297" ht="12" customHeight="1"/>
+    <row r="298" ht="12" customHeight="1"/>
+    <row r="299" ht="12" customHeight="1"/>
+    <row r="300" ht="12" customHeight="1"/>
+    <row r="301" ht="12" customHeight="1"/>
+    <row r="302" ht="12" customHeight="1"/>
+    <row r="303" ht="12" customHeight="1"/>
+    <row r="304" ht="12" customHeight="1"/>
+    <row r="305" ht="12" customHeight="1"/>
+    <row r="306" ht="12" customHeight="1"/>
+    <row r="307" ht="12" customHeight="1"/>
+    <row r="308" ht="12" customHeight="1"/>
+    <row r="309" ht="12" customHeight="1"/>
+    <row r="310" ht="12" customHeight="1"/>
+    <row r="311" ht="12" customHeight="1"/>
+    <row r="312" ht="12" customHeight="1"/>
+    <row r="313" ht="12" customHeight="1"/>
+    <row r="314" ht="12" customHeight="1"/>
+    <row r="315" ht="12" customHeight="1"/>
+    <row r="316" ht="12" customHeight="1"/>
+    <row r="317" ht="12" customHeight="1"/>
+    <row r="318" ht="12" customHeight="1"/>
+    <row r="319" ht="12" customHeight="1"/>
+    <row r="320" ht="12" customHeight="1"/>
+    <row r="321" ht="12" customHeight="1"/>
+    <row r="322" ht="12" customHeight="1"/>
+    <row r="323" ht="12" customHeight="1"/>
+    <row r="324" ht="12" customHeight="1"/>
+    <row r="325" ht="12" customHeight="1"/>
+    <row r="326" ht="12" customHeight="1"/>
+    <row r="327" ht="12" customHeight="1"/>
+    <row r="328" ht="12" customHeight="1"/>
+    <row r="329" ht="12" customHeight="1"/>
+    <row r="330" ht="12" customHeight="1"/>
+    <row r="331" ht="12" customHeight="1"/>
+    <row r="332" ht="12" customHeight="1"/>
+    <row r="333" ht="12" customHeight="1"/>
+    <row r="334" ht="12" customHeight="1"/>
+    <row r="335" ht="12" customHeight="1"/>
+    <row r="336" ht="12" customHeight="1"/>
+    <row r="337" ht="12" customHeight="1"/>
+    <row r="338" ht="12" customHeight="1"/>
+    <row r="339" ht="12" customHeight="1"/>
+    <row r="340" ht="12" customHeight="1"/>
+    <row r="341" ht="12" customHeight="1"/>
+    <row r="342" ht="12" customHeight="1"/>
+    <row r="343" ht="12" customHeight="1"/>
+    <row r="344" ht="12" customHeight="1"/>
+    <row r="345" ht="12" customHeight="1"/>
+    <row r="346" ht="12" customHeight="1"/>
+    <row r="347" ht="12" customHeight="1"/>
+    <row r="348" ht="12" customHeight="1"/>
+    <row r="349" ht="12" customHeight="1"/>
+    <row r="350" ht="12" customHeight="1"/>
+    <row r="351" ht="12" customHeight="1"/>
+    <row r="352" ht="12" customHeight="1"/>
+    <row r="353" ht="12" customHeight="1"/>
+    <row r="354" ht="12" customHeight="1"/>
+    <row r="355" ht="12" customHeight="1"/>
+    <row r="356" ht="12" customHeight="1"/>
+    <row r="357" ht="12" customHeight="1"/>
+    <row r="358" ht="12" customHeight="1"/>
+    <row r="359" ht="12" customHeight="1"/>
+    <row r="360" ht="12" customHeight="1"/>
+    <row r="361" ht="12" customHeight="1"/>
+    <row r="362" ht="12" customHeight="1"/>
+    <row r="363" ht="12" customHeight="1"/>
+    <row r="364" ht="12" customHeight="1"/>
+    <row r="365" ht="12" customHeight="1"/>
+    <row r="366" ht="12" customHeight="1"/>
+    <row r="367" ht="12" customHeight="1"/>
+    <row r="368" ht="12" customHeight="1"/>
+    <row r="369" ht="12" customHeight="1"/>
+    <row r="370" ht="12" customHeight="1"/>
+    <row r="371" ht="12" customHeight="1"/>
+    <row r="372" ht="12" customHeight="1"/>
+    <row r="373" ht="12" customHeight="1"/>
+    <row r="374" ht="12" customHeight="1"/>
+    <row r="375" ht="12" customHeight="1"/>
+    <row r="376" ht="12" customHeight="1"/>
+    <row r="377" ht="12" customHeight="1"/>
+    <row r="378" ht="12" customHeight="1"/>
+    <row r="379" ht="12" customHeight="1"/>
+    <row r="380" ht="12" customHeight="1"/>
+    <row r="381" ht="12" customHeight="1"/>
+    <row r="382" ht="12" customHeight="1"/>
+    <row r="383" ht="12" customHeight="1"/>
+    <row r="384" ht="12" customHeight="1"/>
+    <row r="385" ht="12" customHeight="1"/>
+    <row r="386" ht="12" customHeight="1"/>
+    <row r="387" ht="12" customHeight="1"/>
+    <row r="388" ht="12" customHeight="1"/>
+    <row r="389" ht="12" customHeight="1"/>
+    <row r="390" ht="12" customHeight="1"/>
+    <row r="391" ht="12" customHeight="1"/>
+    <row r="392" ht="12" customHeight="1"/>
+    <row r="393" ht="12" customHeight="1"/>
+    <row r="394" ht="12" customHeight="1"/>
+    <row r="395" ht="12" customHeight="1"/>
+    <row r="396" ht="12" customHeight="1"/>
+    <row r="397" ht="12" customHeight="1"/>
+    <row r="398" ht="12" customHeight="1"/>
+    <row r="399" ht="12" customHeight="1"/>
+    <row r="400" ht="12" customHeight="1"/>
+    <row r="401" ht="12" customHeight="1"/>
+    <row r="402" ht="12" customHeight="1"/>
+    <row r="403" ht="12" customHeight="1"/>
+    <row r="404" ht="12" customHeight="1"/>
+    <row r="405" ht="12" customHeight="1"/>
+    <row r="406" ht="12" customHeight="1"/>
+    <row r="407" ht="12" customHeight="1"/>
+    <row r="408" ht="12" customHeight="1"/>
+    <row r="409" ht="12" customHeight="1"/>
+    <row r="410" ht="12" customHeight="1"/>
+    <row r="411" ht="12" customHeight="1"/>
+    <row r="412" ht="12" customHeight="1"/>
+    <row r="413" ht="12" customHeight="1"/>
+    <row r="414" ht="12" customHeight="1"/>
+    <row r="415" ht="12" customHeight="1"/>
+    <row r="416" ht="12" customHeight="1"/>
+    <row r="417" ht="12" customHeight="1"/>
+    <row r="418" ht="12" customHeight="1"/>
+    <row r="419" ht="12" customHeight="1"/>
+    <row r="420" ht="12" customHeight="1"/>
+    <row r="421" ht="12" customHeight="1"/>
+    <row r="422" ht="12" customHeight="1"/>
+    <row r="423" ht="12" customHeight="1"/>
+    <row r="424" ht="12" customHeight="1"/>
+    <row r="425" ht="12" customHeight="1"/>
+    <row r="426" ht="12" customHeight="1"/>
+    <row r="427" ht="12" customHeight="1"/>
+    <row r="428" ht="12" customHeight="1"/>
+    <row r="429" ht="12" customHeight="1"/>
+    <row r="430" ht="12" customHeight="1"/>
+    <row r="431" ht="12" customHeight="1"/>
+    <row r="432" ht="12" customHeight="1"/>
+    <row r="433" ht="12" customHeight="1"/>
+    <row r="434" ht="12" customHeight="1"/>
+    <row r="435" ht="12" customHeight="1"/>
+    <row r="436" ht="12" customHeight="1"/>
+    <row r="437" ht="12" customHeight="1"/>
+    <row r="438" ht="12" customHeight="1"/>
+    <row r="439" ht="12" customHeight="1"/>
+    <row r="440" ht="12" customHeight="1"/>
+    <row r="441" ht="12" customHeight="1"/>
+    <row r="442" ht="12" customHeight="1"/>
+    <row r="443" ht="12" customHeight="1"/>
+    <row r="444" ht="12" customHeight="1"/>
+    <row r="445" ht="12" customHeight="1"/>
+    <row r="446" ht="12" customHeight="1"/>
+    <row r="447" ht="12" customHeight="1"/>
+    <row r="448" ht="12" customHeight="1"/>
+    <row r="449" ht="12" customHeight="1"/>
+    <row r="450" ht="12" customHeight="1"/>
+    <row r="451" ht="12" customHeight="1"/>
+    <row r="452" ht="12" customHeight="1"/>
+    <row r="453" ht="12" customHeight="1"/>
+    <row r="454" ht="12" customHeight="1"/>
+    <row r="455" ht="12" customHeight="1"/>
+    <row r="456" ht="12" customHeight="1"/>
+    <row r="457" ht="12" customHeight="1"/>
+    <row r="458" ht="12" customHeight="1"/>
+    <row r="459" ht="12" customHeight="1"/>
+    <row r="460" ht="12" customHeight="1"/>
+    <row r="461" ht="12" customHeight="1"/>
+    <row r="462" ht="12" customHeight="1"/>
+    <row r="463" ht="12" customHeight="1"/>
+    <row r="464" ht="12" customHeight="1"/>
+    <row r="465" ht="12" customHeight="1"/>
+    <row r="466" ht="12" customHeight="1"/>
+    <row r="467" ht="12" customHeight="1"/>
+    <row r="468" ht="12" customHeight="1"/>
+    <row r="469" ht="12" customHeight="1"/>
+    <row r="470" ht="12" customHeight="1"/>
+    <row r="471" ht="12" customHeight="1"/>
+    <row r="472" ht="12" customHeight="1"/>
+    <row r="473" ht="12" customHeight="1"/>
+    <row r="474" ht="12" customHeight="1"/>
+    <row r="475" ht="12" customHeight="1"/>
+    <row r="476" ht="12" customHeight="1"/>
+    <row r="477" ht="12" customHeight="1"/>
+    <row r="478" ht="12" customHeight="1"/>
+    <row r="479" ht="12" customHeight="1"/>
+    <row r="480" ht="12" customHeight="1"/>
+    <row r="481" ht="12" customHeight="1"/>
+    <row r="482" ht="12" customHeight="1"/>
+    <row r="483" ht="12" customHeight="1"/>
+    <row r="484" ht="12" customHeight="1"/>
+    <row r="485" ht="12" customHeight="1"/>
+    <row r="486" ht="12" customHeight="1"/>
+    <row r="487" ht="12" customHeight="1"/>
+    <row r="488" ht="12" customHeight="1"/>
+    <row r="489" ht="12" customHeight="1"/>
+    <row r="490" ht="12" customHeight="1"/>
+    <row r="491" ht="12" customHeight="1"/>
+    <row r="492" ht="12" customHeight="1"/>
+    <row r="493" ht="12" customHeight="1"/>
+    <row r="494" ht="12" customHeight="1"/>
+    <row r="495" ht="12" customHeight="1"/>
+    <row r="496" ht="12" customHeight="1"/>
+    <row r="497" ht="12" customHeight="1"/>
+    <row r="498" ht="12" customHeight="1"/>
+    <row r="499" ht="12" customHeight="1"/>
+    <row r="500" ht="12" customHeight="1"/>
+    <row r="501" ht="12" customHeight="1"/>
+    <row r="502" ht="12" customHeight="1"/>
+    <row r="503" ht="12" customHeight="1"/>
+    <row r="504" ht="12" customHeight="1"/>
+    <row r="505" ht="12" customHeight="1"/>
+    <row r="506" ht="12" customHeight="1"/>
+    <row r="507" ht="12" customHeight="1"/>
+    <row r="508" ht="12" customHeight="1"/>
+    <row r="509" ht="12" customHeight="1"/>
+    <row r="510" ht="12" customHeight="1"/>
+    <row r="511" ht="12" customHeight="1"/>
+    <row r="512" ht="12" customHeight="1"/>
+    <row r="513" ht="12" customHeight="1"/>
+    <row r="514" ht="12" customHeight="1"/>
+    <row r="515" ht="12" customHeight="1"/>
+    <row r="516" ht="12" customHeight="1"/>
+    <row r="517" ht="12" customHeight="1"/>
+    <row r="518" ht="12" customHeight="1"/>
+    <row r="519" ht="12" customHeight="1"/>
+    <row r="520" ht="12" customHeight="1"/>
+    <row r="521" ht="12" customHeight="1"/>
+    <row r="522" ht="12" customHeight="1"/>
+    <row r="523" ht="12" customHeight="1"/>
+    <row r="524" ht="12" customHeight="1"/>
+    <row r="525" ht="12" customHeight="1"/>
+    <row r="526" ht="12" customHeight="1"/>
+    <row r="527" ht="12" customHeight="1"/>
+    <row r="528" ht="12" customHeight="1"/>
+    <row r="529" ht="12" customHeight="1"/>
+    <row r="530" ht="12" customHeight="1"/>
+    <row r="531" ht="12" customHeight="1"/>
+    <row r="532" ht="12" customHeight="1"/>
+    <row r="533" ht="12" customHeight="1"/>
+    <row r="534" ht="12" customHeight="1"/>
+    <row r="535" ht="12" customHeight="1"/>
+    <row r="536" ht="12" customHeight="1"/>
+    <row r="537" ht="12" customHeight="1"/>
+    <row r="538" ht="12" customHeight="1"/>
+    <row r="539" ht="12" customHeight="1"/>
+    <row r="540" ht="12" customHeight="1"/>
+    <row r="541" ht="12" customHeight="1"/>
+    <row r="542" ht="12" customHeight="1"/>
+    <row r="543" ht="12" customHeight="1"/>
+    <row r="544" ht="12" customHeight="1"/>
+    <row r="545" ht="12" customHeight="1"/>
+    <row r="546" ht="12" customHeight="1"/>
+    <row r="547" ht="12" customHeight="1"/>
+    <row r="548" ht="12" customHeight="1"/>
+    <row r="549" ht="12" customHeight="1"/>
+    <row r="550" ht="12" customHeight="1"/>
+    <row r="551" ht="12" customHeight="1"/>
+    <row r="552" ht="12" customHeight="1"/>
+    <row r="553" ht="12" customHeight="1"/>
+    <row r="554" ht="12" customHeight="1"/>
+    <row r="555" ht="12" customHeight="1"/>
+    <row r="556" ht="12" customHeight="1"/>
+    <row r="557" ht="12" customHeight="1"/>
+    <row r="558" ht="12" customHeight="1"/>
+    <row r="559" ht="12" customHeight="1"/>
+    <row r="560" ht="12" customHeight="1"/>
+    <row r="561" ht="12" customHeight="1"/>
+    <row r="562" ht="12" customHeight="1"/>
+    <row r="563" ht="12" customHeight="1"/>
+    <row r="564" ht="12" customHeight="1"/>
+    <row r="565" ht="12" customHeight="1"/>
+    <row r="566" ht="12" customHeight="1"/>
+    <row r="567" ht="12" customHeight="1"/>
+    <row r="568" ht="12" customHeight="1"/>
+    <row r="569" ht="12" customHeight="1"/>
+    <row r="570" ht="12" customHeight="1"/>
+    <row r="571" ht="12" customHeight="1"/>
+    <row r="572" ht="12" customHeight="1"/>
+    <row r="573" ht="12" customHeight="1"/>
+    <row r="574" ht="12" customHeight="1"/>
+    <row r="575" ht="12" customHeight="1"/>
+    <row r="576" ht="12" customHeight="1"/>
+    <row r="577" ht="12" customHeight="1"/>
+    <row r="578" ht="12" customHeight="1"/>
+    <row r="579" ht="12" customHeight="1"/>
+    <row r="580" ht="12" customHeight="1"/>
+    <row r="581" ht="12" customHeight="1"/>
+    <row r="582" ht="12" customHeight="1"/>
+    <row r="583" ht="12" customHeight="1"/>
+    <row r="584" ht="12" customHeight="1"/>
+    <row r="585" ht="12" customHeight="1"/>
+    <row r="586" ht="12" customHeight="1"/>
+    <row r="587" ht="12" customHeight="1"/>
+    <row r="588" ht="12" customHeight="1"/>
+    <row r="589" ht="12" customHeight="1"/>
+    <row r="590" ht="12" customHeight="1"/>
+    <row r="591" ht="12" customHeight="1"/>
+    <row r="592" ht="12" customHeight="1"/>
+    <row r="593" ht="12" customHeight="1"/>
+    <row r="594" ht="12" customHeight="1"/>
+    <row r="595" ht="12" customHeight="1"/>
+    <row r="596" ht="12" customHeight="1"/>
+    <row r="597" ht="12" customHeight="1"/>
+    <row r="598" ht="12" customHeight="1"/>
+    <row r="599" ht="12" customHeight="1"/>
+    <row r="600" ht="12" customHeight="1"/>
+    <row r="601" ht="12" customHeight="1"/>
+    <row r="602" ht="12" customHeight="1"/>
+    <row r="603" ht="12" customHeight="1"/>
+    <row r="604" ht="12" customHeight="1"/>
+    <row r="605" ht="12" customHeight="1"/>
+    <row r="606" ht="12" customHeight="1"/>
+    <row r="607" ht="12" customHeight="1"/>
+    <row r="608" ht="12" customHeight="1"/>
+    <row r="609" ht="12" customHeight="1"/>
+    <row r="610" ht="12" customHeight="1"/>
+    <row r="611" ht="12" customHeight="1"/>
+    <row r="612" ht="12" customHeight="1"/>
+    <row r="613" ht="12" customHeight="1"/>
+    <row r="614" ht="12" customHeight="1"/>
+    <row r="615" ht="12" customHeight="1"/>
+    <row r="616" ht="12" customHeight="1"/>
+    <row r="617" ht="12" customHeight="1"/>
+    <row r="618" ht="12" customHeight="1"/>
+    <row r="619" ht="12" customHeight="1"/>
+    <row r="620" ht="12" customHeight="1"/>
+    <row r="621" ht="12" customHeight="1"/>
+    <row r="622" ht="12" customHeight="1"/>
+    <row r="623" ht="12" customHeight="1"/>
+    <row r="624" ht="12" customHeight="1"/>
+    <row r="625" ht="12" customHeight="1"/>
+    <row r="626" ht="12" customHeight="1"/>
+    <row r="627" ht="12" customHeight="1"/>
+    <row r="628" ht="12" customHeight="1"/>
+    <row r="629" ht="12" customHeight="1"/>
+    <row r="630" ht="12" customHeight="1"/>
+    <row r="631" ht="12" customHeight="1"/>
+    <row r="632" ht="12" customHeight="1"/>
+    <row r="633" ht="12" customHeight="1"/>
+    <row r="634" ht="12" customHeight="1"/>
+    <row r="635" ht="12" customHeight="1"/>
+    <row r="636" ht="12" customHeight="1"/>
+    <row r="637" ht="12" customHeight="1"/>
+    <row r="638" ht="12" customHeight="1"/>
+    <row r="639" ht="12" customHeight="1"/>
+    <row r="640" ht="12" customHeight="1"/>
+    <row r="641" ht="12" customHeight="1"/>
+    <row r="642" ht="12" customHeight="1"/>
+    <row r="643" ht="12" customHeight="1"/>
+    <row r="644" ht="12" customHeight="1"/>
+    <row r="645" ht="12" customHeight="1"/>
+    <row r="646" ht="12" customHeight="1"/>
+    <row r="647" ht="12" customHeight="1"/>
+    <row r="648" ht="12" customHeight="1"/>
+    <row r="649" ht="12" customHeight="1"/>
+    <row r="650" ht="12" customHeight="1"/>
+    <row r="651" ht="12" customHeight="1"/>
+    <row r="652" ht="12" customHeight="1"/>
+    <row r="653" ht="12" customHeight="1"/>
+    <row r="654" ht="12" customHeight="1"/>
+    <row r="655" ht="12" customHeight="1"/>
+    <row r="656" ht="12" customHeight="1"/>
+    <row r="657" ht="12" customHeight="1"/>
+    <row r="658" ht="12" customHeight="1"/>
+    <row r="659" ht="12" customHeight="1"/>
+    <row r="660" ht="12" customHeight="1"/>
+    <row r="661" ht="12" customHeight="1"/>
+    <row r="662" ht="12" customHeight="1"/>
+    <row r="663" ht="12" customHeight="1"/>
+    <row r="664" ht="12" customHeight="1"/>
+    <row r="665" ht="12" customHeight="1"/>
+    <row r="666" ht="12" customHeight="1"/>
+    <row r="667" ht="12" customHeight="1"/>
+    <row r="668" ht="12" customHeight="1"/>
+    <row r="669" ht="12" customHeight="1"/>
+    <row r="670" ht="12" customHeight="1"/>
+    <row r="671" ht="12" customHeight="1"/>
+    <row r="672" ht="12" customHeight="1"/>
+    <row r="673" ht="12" customHeight="1"/>
+    <row r="674" ht="12" customHeight="1"/>
+    <row r="675" ht="12" customHeight="1"/>
+    <row r="676" ht="12" customHeight="1"/>
+    <row r="677" ht="12" customHeight="1"/>
+    <row r="678" ht="12" customHeight="1"/>
+    <row r="679" ht="12" customHeight="1"/>
+    <row r="680" ht="12" customHeight="1"/>
+    <row r="681" ht="12" customHeight="1"/>
+    <row r="682" ht="12" customHeight="1"/>
+    <row r="683" ht="12" customHeight="1"/>
+    <row r="684" ht="12" customHeight="1"/>
+    <row r="685" ht="12" customHeight="1"/>
+    <row r="686" ht="12" customHeight="1"/>
+    <row r="687" ht="12" customHeight="1"/>
+    <row r="688" ht="12" customHeight="1"/>
+    <row r="689" ht="12" customHeight="1"/>
+    <row r="690" ht="12" customHeight="1"/>
+    <row r="691" ht="12" customHeight="1"/>
+    <row r="692" ht="12" customHeight="1"/>
+    <row r="693" ht="12" customHeight="1"/>
+    <row r="694" ht="12" customHeight="1"/>
+    <row r="695" ht="12" customHeight="1"/>
+    <row r="696" ht="12" customHeight="1"/>
+    <row r="697" ht="12" customHeight="1"/>
+    <row r="698" ht="12" customHeight="1"/>
+    <row r="699" ht="12" customHeight="1"/>
+    <row r="700" ht="12" customHeight="1"/>
+    <row r="701" ht="12" customHeight="1"/>
+    <row r="702" ht="12" customHeight="1"/>
+    <row r="703" ht="12" customHeight="1"/>
+    <row r="704" ht="12" customHeight="1"/>
+    <row r="705" ht="12" customHeight="1"/>
+    <row r="706" ht="12" customHeight="1"/>
+    <row r="707" ht="12" customHeight="1"/>
+    <row r="708" ht="12" customHeight="1"/>
+    <row r="709" ht="12" customHeight="1"/>
+    <row r="710" ht="12" customHeight="1"/>
+    <row r="711" ht="12" customHeight="1"/>
+    <row r="712" ht="12" customHeight="1"/>
+    <row r="713" ht="12" customHeight="1"/>
+    <row r="714" ht="12" customHeight="1"/>
+    <row r="715" ht="12" customHeight="1"/>
+    <row r="716" ht="12" customHeight="1"/>
+    <row r="717" ht="12" customHeight="1"/>
+    <row r="718" ht="12" customHeight="1"/>
+    <row r="719" ht="12" customHeight="1"/>
+    <row r="720" ht="12" customHeight="1"/>
+    <row r="721" ht="12" customHeight="1"/>
+    <row r="722" ht="12" customHeight="1"/>
+    <row r="723" ht="12" customHeight="1"/>
+    <row r="724" ht="12" customHeight="1"/>
+    <row r="725" ht="12" customHeight="1"/>
+    <row r="726" ht="12" customHeight="1"/>
+    <row r="727" ht="12" customHeight="1"/>
+    <row r="728" ht="12" customHeight="1"/>
+    <row r="729" ht="12" customHeight="1"/>
+    <row r="730" ht="12" customHeight="1"/>
+    <row r="731" ht="12" customHeight="1"/>
+    <row r="732" ht="12" customHeight="1"/>
+    <row r="733" ht="12" customHeight="1"/>
+    <row r="734" ht="12" customHeight="1"/>
+    <row r="735" ht="12" customHeight="1"/>
+    <row r="736" ht="12" customHeight="1"/>
+    <row r="737" ht="12" customHeight="1"/>
+    <row r="738" ht="12" customHeight="1"/>
+    <row r="739" ht="12" customHeight="1"/>
+    <row r="740" ht="12" customHeight="1"/>
+    <row r="741" ht="12" customHeight="1"/>
+    <row r="742" ht="12" customHeight="1"/>
+    <row r="743" ht="12" customHeight="1"/>
+    <row r="744" ht="12" customHeight="1"/>
+    <row r="745" ht="12" customHeight="1"/>
+    <row r="746" ht="12" customHeight="1"/>
+    <row r="747" ht="12" customHeight="1"/>
+    <row r="748" ht="12" customHeight="1"/>
+    <row r="749" ht="12" customHeight="1"/>
+    <row r="750" ht="12" customHeight="1"/>
+    <row r="751" ht="12" customHeight="1"/>
+    <row r="752" ht="12" customHeight="1"/>
+    <row r="753" ht="12" customHeight="1"/>
+    <row r="754" ht="12" customHeight="1"/>
+    <row r="755" ht="12" customHeight="1"/>
+    <row r="756" ht="12" customHeight="1"/>
+    <row r="757" ht="12" customHeight="1"/>
+    <row r="758" ht="12" customHeight="1"/>
+    <row r="759" ht="12" customHeight="1"/>
+    <row r="760" ht="12" customHeight="1"/>
+    <row r="761" ht="12" customHeight="1"/>
+    <row r="762" ht="12" customHeight="1"/>
+    <row r="763" ht="12" customHeight="1"/>
+    <row r="764" ht="12" customHeight="1"/>
+    <row r="765" ht="12" customHeight="1"/>
+    <row r="766" ht="12" customHeight="1"/>
+    <row r="767" ht="12" customHeight="1"/>
+    <row r="768" ht="12" customHeight="1"/>
+    <row r="769" ht="12" customHeight="1"/>
+    <row r="770" ht="12" customHeight="1"/>
+    <row r="771" ht="12" customHeight="1"/>
+    <row r="772" ht="12" customHeight="1"/>
+    <row r="773" ht="12" customHeight="1"/>
+    <row r="774" ht="12" customHeight="1"/>
+    <row r="775" ht="12" customHeight="1"/>
+    <row r="776" ht="12" customHeight="1"/>
+    <row r="777" ht="12" customHeight="1"/>
+    <row r="778" ht="12" customHeight="1"/>
+    <row r="779" ht="12" customHeight="1"/>
+    <row r="780" ht="12" customHeight="1"/>
+    <row r="781" ht="12" customHeight="1"/>
+    <row r="782" ht="12" customHeight="1"/>
+    <row r="783" ht="12" customHeight="1"/>
+    <row r="784" ht="12" customHeight="1"/>
+    <row r="785" ht="12" customHeight="1"/>
+    <row r="786" ht="12" customHeight="1"/>
+    <row r="787" ht="12" customHeight="1"/>
+    <row r="788" ht="12" customHeight="1"/>
+    <row r="789" ht="12" customHeight="1"/>
+    <row r="790" ht="12" customHeight="1"/>
+    <row r="791" ht="12" customHeight="1"/>
+    <row r="792" ht="12" customHeight="1"/>
+    <row r="793" ht="12" customHeight="1"/>
+    <row r="794" ht="12" customHeight="1"/>
+    <row r="795" ht="12" customHeight="1"/>
+    <row r="796" ht="12" customHeight="1"/>
+    <row r="797" ht="12" customHeight="1"/>
+    <row r="798" ht="12" customHeight="1"/>
+    <row r="799" ht="12" customHeight="1"/>
+    <row r="800" ht="12" customHeight="1"/>
+    <row r="801" ht="12" customHeight="1"/>
+    <row r="802" ht="12" customHeight="1"/>
+    <row r="803" ht="12" customHeight="1"/>
+    <row r="804" ht="12" customHeight="1"/>
+    <row r="805" ht="12" customHeight="1"/>
+    <row r="806" ht="12" customHeight="1"/>
+    <row r="807" ht="12" customHeight="1"/>
+    <row r="808" ht="12" customHeight="1"/>
+    <row r="809" ht="12" customHeight="1"/>
+    <row r="810" ht="12" customHeight="1"/>
+    <row r="811" ht="12" customHeight="1"/>
+    <row r="812" ht="12" customHeight="1"/>
+    <row r="813" ht="12" customHeight="1"/>
+    <row r="814" ht="12" customHeight="1"/>
+    <row r="815" ht="12" customHeight="1"/>
+    <row r="816" ht="12" customHeight="1"/>
+    <row r="817" ht="12" customHeight="1"/>
+    <row r="818" ht="12" customHeight="1"/>
+    <row r="819" ht="12" customHeight="1"/>
+    <row r="820" ht="12" customHeight="1"/>
+    <row r="821" ht="12" customHeight="1"/>
+    <row r="822" ht="12" customHeight="1"/>
+    <row r="823" ht="12" customHeight="1"/>
+    <row r="824" ht="12" customHeight="1"/>
+    <row r="825" ht="12" customHeight="1"/>
+    <row r="826" ht="12" customHeight="1"/>
+    <row r="827" ht="12" customHeight="1"/>
+    <row r="828" ht="12" customHeight="1"/>
+    <row r="829" ht="12" customHeight="1"/>
+    <row r="830" ht="12" customHeight="1"/>
+    <row r="831" ht="12" customHeight="1"/>
+    <row r="832" ht="12" customHeight="1"/>
+    <row r="833" ht="12" customHeight="1"/>
+    <row r="834" ht="12" customHeight="1"/>
+    <row r="835" ht="12" customHeight="1"/>
+    <row r="836" ht="12" customHeight="1"/>
+    <row r="837" ht="12" customHeight="1"/>
+    <row r="838" ht="12" customHeight="1"/>
+    <row r="839" ht="12" customHeight="1"/>
+    <row r="840" ht="12" customHeight="1"/>
+    <row r="841" ht="12" customHeight="1"/>
+    <row r="842" ht="12" customHeight="1"/>
+    <row r="843" ht="12" customHeight="1"/>
+    <row r="844" ht="12" customHeight="1"/>
+    <row r="845" ht="12" customHeight="1"/>
+    <row r="846" ht="12" customHeight="1"/>
+    <row r="847" ht="12" customHeight="1"/>
+    <row r="848" ht="12" customHeight="1"/>
+    <row r="849" ht="12" customHeight="1"/>
+    <row r="850" ht="12" customHeight="1"/>
+    <row r="851" ht="12" customHeight="1"/>
+    <row r="852" ht="12" customHeight="1"/>
+    <row r="853" ht="12" customHeight="1"/>
+    <row r="854" ht="12" customHeight="1"/>
+    <row r="855" ht="12" customHeight="1"/>
+    <row r="856" ht="12" customHeight="1"/>
+    <row r="857" ht="12" customHeight="1"/>
+    <row r="858" ht="12" customHeight="1"/>
+    <row r="859" ht="12" customHeight="1"/>
+    <row r="860" ht="12" customHeight="1"/>
+    <row r="861" ht="12" customHeight="1"/>
+    <row r="862" ht="12" customHeight="1"/>
+    <row r="863" ht="12" customHeight="1"/>
+    <row r="864" ht="12" customHeight="1"/>
+    <row r="865" ht="12" customHeight="1"/>
+    <row r="866" ht="12" customHeight="1"/>
+    <row r="867" ht="12" customHeight="1"/>
+    <row r="868" ht="12" customHeight="1"/>
+    <row r="869" ht="12" customHeight="1"/>
+    <row r="870" ht="12" customHeight="1"/>
+    <row r="871" ht="12" customHeight="1"/>
+    <row r="872" ht="12" customHeight="1"/>
+    <row r="873" ht="12" customHeight="1"/>
+    <row r="874" ht="12" customHeight="1"/>
+    <row r="875" ht="12" customHeight="1"/>
+    <row r="876" ht="12" customHeight="1"/>
+    <row r="877" ht="12" customHeight="1"/>
+    <row r="878" ht="12" customHeight="1"/>
+    <row r="879" ht="12" customHeight="1"/>
+    <row r="880" ht="12" customHeight="1"/>
+    <row r="881" ht="12" customHeight="1"/>
+    <row r="882" ht="12" customHeight="1"/>
+    <row r="883" ht="12" customHeight="1"/>
+    <row r="884" ht="12" customHeight="1"/>
+    <row r="885" ht="12" customHeight="1"/>
+    <row r="886" ht="12" customHeight="1"/>
+    <row r="887" ht="12" customHeight="1"/>
+    <row r="888" ht="12" customHeight="1"/>
+    <row r="889" ht="12" customHeight="1"/>
+    <row r="890" ht="12" customHeight="1"/>
+    <row r="891" ht="12" customHeight="1"/>
+    <row r="892" ht="12" customHeight="1"/>
+    <row r="893" ht="12" customHeight="1"/>
+    <row r="894" ht="12" customHeight="1"/>
+    <row r="895" ht="12" customHeight="1"/>
+    <row r="896" ht="12" customHeight="1"/>
+    <row r="897" ht="12" customHeight="1"/>
+    <row r="898" ht="12" customHeight="1"/>
+    <row r="899" ht="12" customHeight="1"/>
+    <row r="900" ht="12" customHeight="1"/>
+    <row r="901" ht="12" customHeight="1"/>
+    <row r="902" ht="12" customHeight="1"/>
+    <row r="903" ht="12" customHeight="1"/>
+    <row r="904" ht="12" customHeight="1"/>
+    <row r="905" ht="12" customHeight="1"/>
+    <row r="906" ht="12" customHeight="1"/>
+    <row r="907" ht="12" customHeight="1"/>
+    <row r="908" ht="12" customHeight="1"/>
+    <row r="909" ht="12" customHeight="1"/>
+    <row r="910" ht="12" customHeight="1"/>
+    <row r="911" ht="12" customHeight="1"/>
+    <row r="912" ht="12" customHeight="1"/>
+    <row r="913" ht="12" customHeight="1"/>
+    <row r="914" ht="12" customHeight="1"/>
+    <row r="915" ht="12" customHeight="1"/>
+    <row r="916" ht="12" customHeight="1"/>
+    <row r="917" ht="12" customHeight="1"/>
+    <row r="918" ht="12" customHeight="1"/>
+    <row r="919" ht="12" customHeight="1"/>
+    <row r="920" ht="12" customHeight="1"/>
+    <row r="921" ht="12" customHeight="1"/>
+    <row r="922" ht="12" customHeight="1"/>
+    <row r="923" ht="12" customHeight="1"/>
+    <row r="924" ht="12" customHeight="1"/>
+    <row r="925" ht="12" customHeight="1"/>
+    <row r="926" ht="12" customHeight="1"/>
+    <row r="927" ht="12" customHeight="1"/>
+    <row r="928" ht="12" customHeight="1"/>
+    <row r="929" ht="12" customHeight="1"/>
+    <row r="930" ht="12" customHeight="1"/>
+    <row r="931" ht="12" customHeight="1"/>
+    <row r="932" ht="12" customHeight="1"/>
+    <row r="933" ht="12" customHeight="1"/>
+    <row r="934" ht="12" customHeight="1"/>
+    <row r="935" ht="12" customHeight="1"/>
+    <row r="936" ht="12" customHeight="1"/>
+    <row r="937" ht="12" customHeight="1"/>
+    <row r="938" ht="12" customHeight="1"/>
+    <row r="939" ht="12" customHeight="1"/>
+    <row r="940" ht="12" customHeight="1"/>
+    <row r="941" ht="12" customHeight="1"/>
+    <row r="942" ht="12" customHeight="1"/>
+    <row r="943" ht="12" customHeight="1"/>
+    <row r="944" ht="12" customHeight="1"/>
+    <row r="945" ht="12" customHeight="1"/>
+    <row r="946" ht="12" customHeight="1"/>
+    <row r="947" ht="12" customHeight="1"/>
+    <row r="948" ht="12" customHeight="1"/>
+    <row r="949" ht="12" customHeight="1"/>
+    <row r="950" ht="12" customHeight="1"/>
+    <row r="951" ht="12" customHeight="1"/>
+    <row r="952" ht="12" customHeight="1"/>
+    <row r="953" ht="12" customHeight="1"/>
+    <row r="954" ht="12" customHeight="1"/>
+    <row r="955" ht="12" customHeight="1"/>
+    <row r="956" ht="12" customHeight="1"/>
+    <row r="957" ht="12" customHeight="1"/>
+    <row r="958" ht="12" customHeight="1"/>
+    <row r="959" ht="12" customHeight="1"/>
+    <row r="960" ht="12" customHeight="1"/>
+    <row r="961" ht="12" customHeight="1"/>
+    <row r="962" ht="12" customHeight="1"/>
+    <row r="963" ht="12" customHeight="1"/>
+    <row r="964" ht="12" customHeight="1"/>
+    <row r="965" ht="12" customHeight="1"/>
+    <row r="966" ht="12" customHeight="1"/>
+    <row r="967" ht="12" customHeight="1"/>
+    <row r="968" ht="12" customHeight="1"/>
+    <row r="969" ht="12" customHeight="1"/>
+    <row r="970" ht="12" customHeight="1"/>
+    <row r="971" ht="12" customHeight="1"/>
+    <row r="972" ht="12" customHeight="1"/>
+    <row r="973" ht="12" customHeight="1"/>
+    <row r="974" ht="12" customHeight="1"/>
+    <row r="975" ht="12" customHeight="1"/>
+    <row r="976" ht="12" customHeight="1"/>
+    <row r="977" ht="12" customHeight="1"/>
+    <row r="978" ht="12" customHeight="1"/>
+    <row r="979" ht="12" customHeight="1"/>
+    <row r="980" ht="12" customHeight="1"/>
+    <row r="981" ht="12" customHeight="1"/>
+    <row r="982" ht="12" customHeight="1"/>
+    <row r="983" ht="12" customHeight="1"/>
+    <row r="984" ht="12" customHeight="1"/>
+    <row r="985" ht="12" customHeight="1"/>
+    <row r="986" ht="12" customHeight="1"/>
+    <row r="987" ht="12" customHeight="1"/>
+    <row r="988" ht="12" customHeight="1"/>
+    <row r="989" ht="12" customHeight="1"/>
+    <row r="990" ht="12" customHeight="1"/>
+    <row r="991" ht="12" customHeight="1"/>
+    <row r="992" ht="12" customHeight="1"/>
+    <row r="993" ht="12" customHeight="1"/>
+    <row r="994" ht="12" customHeight="1"/>
+    <row r="995" ht="12" customHeight="1"/>
+    <row r="996" ht="12" customHeight="1"/>
+    <row r="997" ht="12" customHeight="1"/>
+    <row r="998" ht="12" customHeight="1"/>
+    <row r="999" ht="12" customHeight="1"/>
+    <row r="1000" ht="12" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9584C1FB-8309-4FF5-81F6-EB9C6421B4E2}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>

</xml_diff>